<commit_message>
about to start redoing opensim for mediapipe
</commit_message>
<xml_diff>
--- a/FMC_to_trc/trajectory_map.xlsx
+++ b/FMC_to_trc/trajectory_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mac Prible\Box\Research\FMC_projects\FMC_to_trc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C69EBE6-133B-462F-89A3-7B856EADCE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B70069C-84BB-4A0F-9B3E-C69BC564590A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
-  <si>
-    <t>mediapipe_tracked_point_names =  [</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>    "nose",</t>
   </si>
@@ -263,9 +260,6 @@
   </si>
   <si>
     <t>    "left_hand_pinky_finger_tip",</t>
-  </si>
-  <si>
-    <t>    ]</t>
   </si>
 </sst>
 </file>
@@ -593,700 +587,691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C8:D84"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>A1+1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <f>C9+1</f>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ref="A3:A66" si="0">A2+1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <f t="shared" ref="C11:C74" si="0">C10+1</f>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <f t="shared" si="0"/>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <f t="shared" si="0"/>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="1" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <f t="shared" si="0"/>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="1" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <f t="shared" si="0"/>
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <f t="shared" si="0"/>
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="1" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <f t="shared" si="0"/>
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="1" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <f t="shared" si="0"/>
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="1" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <f t="shared" si="0"/>
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="1" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <f t="shared" si="0"/>
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="1" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <f t="shared" si="0"/>
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="1" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22">
-        <f t="shared" si="0"/>
+      <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="1" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23">
-        <f t="shared" si="0"/>
+      <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="1" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24">
-        <f t="shared" si="0"/>
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="1" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <f t="shared" si="0"/>
+      <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="1" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <f t="shared" si="0"/>
+      <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="1" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <f t="shared" si="0"/>
+      <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="1" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <f t="shared" si="0"/>
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="1" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29">
-        <f t="shared" si="0"/>
+      <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="1" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C30">
-        <f t="shared" si="0"/>
+      <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="1" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <f t="shared" si="0"/>
+      <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="1" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C32">
-        <f t="shared" si="0"/>
+      <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="1" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33">
-        <f t="shared" si="0"/>
+      <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="1" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <f t="shared" si="0"/>
+      <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="1" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35">
-        <f t="shared" si="0"/>
+      <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="1" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36">
-        <f t="shared" si="0"/>
+      <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="1" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37">
-        <f t="shared" si="0"/>
+      <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="1" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38">
-        <f t="shared" si="0"/>
+      <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="1" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39">
-        <f t="shared" si="0"/>
+      <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="1" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40">
-        <f t="shared" si="0"/>
+      <c r="B32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="1" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41">
-        <f t="shared" si="0"/>
+      <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="1" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42">
-        <f t="shared" si="0"/>
+      <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="1" t="s">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C43">
-        <f t="shared" si="0"/>
+      <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="1" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C44">
-        <f t="shared" si="0"/>
+      <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D44" s="1" t="s">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45">
-        <f t="shared" si="0"/>
+      <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D45" s="1" t="s">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46">
-        <f t="shared" si="0"/>
+      <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="1" t="s">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C47">
-        <f t="shared" si="0"/>
+      <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="1" t="s">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C48">
-        <f t="shared" si="0"/>
+      <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="1" t="s">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49">
-        <f t="shared" si="0"/>
+      <c r="B41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D49" s="1" t="s">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50">
-        <f t="shared" si="0"/>
+      <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D50" s="1" t="s">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51">
-        <f t="shared" si="0"/>
+      <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D51" s="1" t="s">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52">
-        <f t="shared" si="0"/>
+      <c r="B44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D52" s="1" t="s">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53">
-        <f t="shared" si="0"/>
+      <c r="B45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D53" s="1" t="s">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54">
-        <f t="shared" si="0"/>
+      <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D54" s="1" t="s">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55">
-        <f t="shared" si="0"/>
+      <c r="B47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D55" s="1" t="s">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56">
-        <f t="shared" si="0"/>
+      <c r="B48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D56" s="1" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57">
-        <f t="shared" si="0"/>
+      <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D57" s="1" t="s">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58">
-        <f t="shared" si="0"/>
+      <c r="B50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D58" s="1" t="s">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59">
-        <f t="shared" si="0"/>
+      <c r="B51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D59" s="1" t="s">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60">
-        <f t="shared" si="0"/>
+      <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D60" s="1" t="s">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61">
-        <f t="shared" si="0"/>
+      <c r="B53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D61" s="1" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62">
-        <f t="shared" si="0"/>
+      <c r="B54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D62" s="1" t="s">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63">
-        <f t="shared" si="0"/>
+      <c r="B55" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D63" s="1" t="s">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64">
-        <f t="shared" si="0"/>
+      <c r="B56" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D64" s="1" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65">
-        <f t="shared" si="0"/>
+      <c r="B57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D65" s="1" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66">
-        <f t="shared" si="0"/>
+      <c r="B58" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D66" s="1" t="s">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67">
-        <f t="shared" si="0"/>
+      <c r="B59" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D67" s="1" t="s">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68">
-        <f t="shared" si="0"/>
+      <c r="B60" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D68" s="1" t="s">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69">
-        <f t="shared" si="0"/>
+      <c r="B61" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D69" s="1" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70">
-        <f t="shared" si="0"/>
+      <c r="B62" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D70" s="1" t="s">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71">
-        <f t="shared" si="0"/>
+      <c r="B63" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D71" s="1" t="s">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72">
-        <f t="shared" si="0"/>
+      <c r="B64" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D72" s="1" t="s">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73">
-        <f t="shared" si="0"/>
+      <c r="B65" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D73" s="1" t="s">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74">
-        <f t="shared" si="0"/>
+      <c r="B66" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D74" s="1" t="s">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" ref="A67:A75" si="1">A66+1</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75">
-        <f t="shared" ref="C75:C83" si="1">C74+1</f>
+      <c r="B67" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77">
+      <c r="B68" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78">
+      <c r="B69" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79">
+      <c r="B70" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80">
+      <c r="B71" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81">
+      <c r="B72" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82">
+      <c r="B73" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83">
+      <c r="B74" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="B75" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>